<commit_message>
Standardize workflows related to delete entities
</commit_message>
<xml_diff>
--- a/Config/JA/アセット.xlsx
+++ b/Config/JA/アセット.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA620124-DDBE-43DA-AA55-D984E0468758}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2328731-8BDD-442E-9D91-4B3D20829B37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2390,25 +2390,23 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
+      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B5" s="3"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
@@ -2417,48 +2415,48 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B7" s="3"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B8" s="3"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B9" s="3"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B10" s="3"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B11" s="3"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B12" s="3"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B13" s="3"/>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Handle cases when the user closes the Custom Input activity without submitting the form
</commit_message>
<xml_diff>
--- a/Config/JA/アセット.xlsx
+++ b/Config/JA/アセット.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Config\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A725A5-4FA3-46D0-85B1-F82C0405D3B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1221C6AD-8395-4240-B4A4-E8579058F408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2437,6 +2437,8 @@
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
@@ -2453,7 +2455,6 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B14" s="3"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
@@ -2467,162 +2468,162 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17" s="3"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B18" s="3"/>
+      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="3"/>
+      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="3"/>
+      <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="3"/>
+      <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="3"/>
+      <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="3"/>
+      <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B24" s="3"/>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B25" s="3"/>
+      <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B26" s="3"/>
+      <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="3"/>
+      <c r="D27" s="1"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="3"/>
+      <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="3"/>
+      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B30" s="3"/>
+      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="3"/>
+      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C32" s="1"/>
-      <c r="D32" s="2"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="3"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" s="3"/>
+      <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" s="3"/>
+      <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C40" s="1"/>
       <c r="D40" s="2"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C41" s="1"/>
       <c r="D41" s="2"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C42" s="1"/>
       <c r="D42" s="2"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C44" s="1"/>
       <c r="D44" s="2"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C45" s="1"/>
       <c r="D45" s="2"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C46" s="1"/>
       <c r="D46" s="2"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C48" s="1"/>
       <c r="D48" s="2"/>
       <c r="E48" s="1"/>

</xml_diff>